<commit_message>
Fixed RPI table display, many, many bugs
</commit_message>
<xml_diff>
--- a/data/Prep_RPI.xlsx
+++ b/data/Prep_RPI.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="295">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="479" uniqueCount="294">
   <si>
     <t>School Name</t>
   </si>
@@ -139,9 +139,6 @@
   </si>
   <si>
     <t>andrewbelica@gmail.com</t>
-  </si>
-  <si>
-    <t>Phillips Academy Andover</t>
   </si>
   <si>
     <t>smoreland@andover.edu</t>
@@ -1445,7 +1442,7 @@
   <dimension ref="A1:M1001"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="A1:C11"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1750,7 +1747,7 @@
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="33" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B11" s="28">
         <v>2017</v>
@@ -1776,7 +1773,7 @@
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
-        <v>37</v>
+        <v>210</v>
       </c>
       <c r="B12" s="28">
         <v>2017</v>
@@ -1786,7 +1783,7 @@
         <v>Phillips Andover Academy Boys Lacrosse</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E12" s="14"/>
       <c r="F12" s="14"/>
@@ -1802,7 +1799,7 @@
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B13" s="28">
         <v>2017</v>
@@ -1812,16 +1809,16 @@
         <v>Brunswick School Boys Lacrosse</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="F13" s="7" t="s">
+      <c r="G13" s="7" t="s">
         <v>42</v>
-      </c>
-      <c r="G13" s="7" t="s">
-        <v>43</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7" t="s">
@@ -1834,7 +1831,7 @@
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="28">
         <v>2017</v>
@@ -1844,16 +1841,16 @@
         <v>Avon Old Farms Boys Lacrosse</v>
       </c>
       <c r="D14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E14" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="E14" s="7" t="s">
+      <c r="F14" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="G14" s="7" t="s">
         <v>47</v>
-      </c>
-      <c r="G14" s="7" t="s">
-        <v>48</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7" t="s">
@@ -1866,7 +1863,7 @@
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="28">
         <v>2017</v>
@@ -1876,10 +1873,10 @@
         <v>Taft School Boys Lacrosse</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>50</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>51</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="14"/>
@@ -1894,7 +1891,7 @@
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B16" s="28">
         <v>2017</v>
@@ -1904,10 +1901,10 @@
         <v>Albany Academy Boys Lacrosse</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>53</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>54</v>
       </c>
       <c r="F16" s="14"/>
       <c r="G16" s="14"/>
@@ -1922,7 +1919,7 @@
     </row>
     <row r="17" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B17" s="28">
         <v>2017</v>
@@ -1932,10 +1929,10 @@
         <v>Proctor Academy Boys Lacrosse</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="14"/>
@@ -1950,7 +1947,7 @@
     </row>
     <row r="18" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B18" s="28">
         <v>2017</v>
@@ -1960,7 +1957,7 @@
         <v>Milton Academy Boys Lacrosse</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E18" s="14"/>
       <c r="F18" s="14"/>
@@ -1976,7 +1973,7 @@
     </row>
     <row r="19" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B19" s="28">
         <v>2017</v>
@@ -1986,10 +1983,10 @@
         <v>New Hampton School Boys Lacrosse</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="E19" s="7" t="s">
         <v>61</v>
-      </c>
-      <c r="E19" s="7" t="s">
-        <v>62</v>
       </c>
       <c r="F19" s="14"/>
       <c r="G19" s="14"/>
@@ -2004,7 +2001,7 @@
     </row>
     <row r="20" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="28">
         <v>2017</v>
@@ -2014,10 +2011,10 @@
         <v>Winchendon School Boys Lacrosse</v>
       </c>
       <c r="D20" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="7" t="s">
         <v>64</v>
-      </c>
-      <c r="E20" s="7" t="s">
-        <v>65</v>
       </c>
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
@@ -2032,7 +2029,7 @@
     </row>
     <row r="21" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B21" s="28">
         <v>2017</v>
@@ -2042,7 +2039,7 @@
         <v>St. Sebastian's Academy Boys Lacrosse</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E21" s="14"/>
       <c r="F21" s="14"/>
@@ -2058,7 +2055,7 @@
     </row>
     <row r="22" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B22" s="28">
         <v>2017</v>
@@ -2068,10 +2065,10 @@
         <v>Loomis-Chaffee Boys Lacrosse</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="7" t="s">
         <v>69</v>
-      </c>
-      <c r="E22" s="7" t="s">
-        <v>70</v>
       </c>
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
@@ -2086,7 +2083,7 @@
     </row>
     <row r="23" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B23" s="28">
         <v>2017</v>
@@ -2096,13 +2093,13 @@
         <v>Tabor Academy Boys Lacrosse</v>
       </c>
       <c r="D23" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E23" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="E23" s="7" t="s">
+      <c r="F23" s="7" t="s">
         <v>73</v>
-      </c>
-      <c r="F23" s="7" t="s">
-        <v>74</v>
       </c>
       <c r="G23" s="14"/>
       <c r="H23" s="14"/>
@@ -2116,7 +2113,7 @@
     </row>
     <row r="24" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B24" s="28">
         <v>2017</v>
@@ -2126,10 +2123,10 @@
         <v>Tilton School Boys Lacrosse</v>
       </c>
       <c r="D24" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E24" s="7" t="s">
         <v>76</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>77</v>
       </c>
       <c r="F24" s="14"/>
       <c r="G24" s="14"/>
@@ -2144,7 +2141,7 @@
     </row>
     <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B25" s="28">
         <v>2017</v>
@@ -2154,7 +2151,7 @@
         <v>Kent School Boys Lacrosse</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="14"/>
@@ -2170,7 +2167,7 @@
     </row>
     <row r="26" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B26" s="28">
         <v>2017</v>
@@ -2180,13 +2177,13 @@
         <v>Cushing Academy Boys Lacrosse</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>82</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>83</v>
       </c>
       <c r="G26" s="14"/>
       <c r="H26" s="14"/>
@@ -2200,7 +2197,7 @@
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B27" s="28">
         <v>2017</v>
@@ -2210,7 +2207,7 @@
         <v>Pomfret School Boys Lacrosse</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="14"/>
       <c r="F27" s="14"/>
@@ -2226,7 +2223,7 @@
     </row>
     <row r="28" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B28" s="28">
         <v>2017</v>
@@ -2236,7 +2233,7 @@
         <v>Berkshire School Boys Lacrosse</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E28" s="14"/>
       <c r="F28" s="14"/>
@@ -2252,7 +2249,7 @@
     </row>
     <row r="29" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B29" s="28">
         <v>2017</v>
@@ -2262,7 +2259,7 @@
         <v>Holderness School Boys Lacrosse</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -2278,7 +2275,7 @@
     </row>
     <row r="30" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B30" s="28">
         <v>2017</v>
@@ -2288,19 +2285,19 @@
         <v>Wesminster School Boys Lacrosse</v>
       </c>
       <c r="D30" s="7" t="s">
+        <v>90</v>
+      </c>
+      <c r="E30" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="E30" s="7" t="s">
+      <c r="F30" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="G30" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="G30" s="7" t="s">
+      <c r="H30" s="7" t="s">
         <v>94</v>
-      </c>
-      <c r="H30" s="7" t="s">
-        <v>95</v>
       </c>
       <c r="I30" s="7" t="s">
         <v>8</v>
@@ -2312,7 +2309,7 @@
     </row>
     <row r="31" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B31" s="28">
         <v>2017</v>
@@ -2322,7 +2319,7 @@
         <v>Roxbury Latin School Boys Lacrosse</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E31" s="14"/>
       <c r="F31" s="14"/>
@@ -2338,7 +2335,7 @@
     </row>
     <row r="32" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B32" s="28">
         <v>2017</v>
@@ -2348,13 +2345,13 @@
         <v>Millbrook School Boys Lacrosse</v>
       </c>
       <c r="D32" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="E32" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="E32" s="7" t="s">
+      <c r="F32" s="7" t="s">
         <v>100</v>
-      </c>
-      <c r="F32" s="7" t="s">
-        <v>101</v>
       </c>
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
@@ -2368,7 +2365,7 @@
     </row>
     <row r="33" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B33" s="28">
         <v>2017</v>
@@ -2378,10 +2375,10 @@
         <v>Williston-Northampton Boys Lacrosse</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>103</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>104</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="14"/>
@@ -2396,7 +2393,7 @@
     </row>
     <row r="34" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B34" s="28">
         <v>2017</v>
@@ -2406,13 +2403,13 @@
         <v>Deerfield Academy Boys Lacrosse</v>
       </c>
       <c r="D34" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="E34" s="7" t="s">
         <v>106</v>
       </c>
-      <c r="E34" s="7" t="s">
+      <c r="F34" s="7" t="s">
         <v>107</v>
-      </c>
-      <c r="F34" s="7" t="s">
-        <v>108</v>
       </c>
       <c r="G34" s="14"/>
       <c r="H34" s="14"/>
@@ -2426,7 +2423,7 @@
     </row>
     <row r="35" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B35" s="28">
         <v>2017</v>
@@ -2436,10 +2433,10 @@
         <v>Noble &amp; Greenough Boys Lacrosse</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>110</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>111</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="14"/>
@@ -2454,7 +2451,7 @@
     </row>
     <row r="36" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B36" s="28">
         <v>2017</v>
@@ -2464,7 +2461,7 @@
         <v>Hotchkiss School Boys Lacrosse</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -2480,7 +2477,7 @@
     </row>
     <row r="37" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B37" s="28">
         <v>2017</v>
@@ -2490,10 +2487,10 @@
         <v>St. Paul's Boys Lacrosse</v>
       </c>
       <c r="D37" s="7" t="s">
+        <v>114</v>
+      </c>
+      <c r="E37" s="7" t="s">
         <v>115</v>
-      </c>
-      <c r="E37" s="7" t="s">
-        <v>116</v>
       </c>
       <c r="F37" s="14"/>
       <c r="G37" s="14"/>
@@ -2508,7 +2505,7 @@
     </row>
     <row r="38" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B38" s="28">
         <v>2017</v>
@@ -2518,10 +2515,10 @@
         <v>Governor's Academy Boys Lacrosse</v>
       </c>
       <c r="D38" s="7" t="s">
+        <v>117</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>118</v>
-      </c>
-      <c r="E38" s="7" t="s">
-        <v>119</v>
       </c>
       <c r="F38" s="14"/>
       <c r="G38" s="14"/>
@@ -2536,7 +2533,7 @@
     </row>
     <row r="39" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B39" s="28">
         <v>2017</v>
@@ -2546,13 +2543,13 @@
         <v>Groton School Boys Lacrosse</v>
       </c>
       <c r="D39" s="7" t="s">
+        <v>120</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>121</v>
       </c>
-      <c r="E39" s="7" t="s">
+      <c r="F39" s="7" t="s">
         <v>122</v>
-      </c>
-      <c r="F39" s="7" t="s">
-        <v>123</v>
       </c>
       <c r="G39" s="14"/>
       <c r="H39" s="14"/>
@@ -2566,7 +2563,7 @@
     </row>
     <row r="40" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B40" s="28">
         <v>2017</v>
@@ -2576,7 +2573,7 @@
         <v>St. Mark's School Boys Lacrosse</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -2592,7 +2589,7 @@
     </row>
     <row r="41" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B41" s="28">
         <v>2017</v>
@@ -2602,13 +2599,13 @@
         <v>Choate Boys Lacrosse</v>
       </c>
       <c r="D41" s="7" t="s">
+        <v>126</v>
+      </c>
+      <c r="E41" s="7" t="s">
         <v>127</v>
       </c>
-      <c r="E41" s="7" t="s">
+      <c r="F41" s="7" t="s">
         <v>128</v>
-      </c>
-      <c r="F41" s="7" t="s">
-        <v>129</v>
       </c>
       <c r="G41" s="14"/>
       <c r="H41" s="14"/>
@@ -2622,7 +2619,7 @@
     </row>
     <row r="42" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B42" s="28">
         <v>2017</v>
@@ -2632,13 +2629,13 @@
         <v>BB&amp;N Boys Lacrosse</v>
       </c>
       <c r="D42" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>131</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>132</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>133</v>
       </c>
       <c r="G42" s="14"/>
       <c r="H42" s="14"/>
@@ -2652,7 +2649,7 @@
     </row>
     <row r="43" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B43" s="28">
         <v>2017</v>
@@ -2662,10 +2659,10 @@
         <v>Hebron Academy Boys Lacrosse</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>135</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>136</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="14"/>
@@ -2680,7 +2677,7 @@
     </row>
     <row r="44" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B44" s="28">
         <v>2017</v>
@@ -2690,13 +2687,13 @@
         <v>Trinity-Pawling Boys Lacrosse</v>
       </c>
       <c r="D44" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="E44" s="7" t="s">
         <v>138</v>
       </c>
-      <c r="E44" s="7" t="s">
+      <c r="F44" s="7" t="s">
         <v>139</v>
-      </c>
-      <c r="F44" s="7" t="s">
-        <v>140</v>
       </c>
       <c r="G44" s="14"/>
       <c r="H44" s="14"/>
@@ -2710,7 +2707,7 @@
     </row>
     <row r="45" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B45" s="28">
         <v>2017</v>
@@ -2720,13 +2717,13 @@
         <v>Brooks School Boys Lacrosse</v>
       </c>
       <c r="D45" s="7" t="s">
+        <v>141</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>142</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>143</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>144</v>
       </c>
       <c r="G45" s="14"/>
       <c r="H45" s="14"/>
@@ -2740,7 +2737,7 @@
     </row>
     <row r="46" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B46" s="28">
         <v>2017</v>
@@ -2750,13 +2747,13 @@
         <v>Northfield - Mt Hermon Boys Lacrosse</v>
       </c>
       <c r="D46" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="F46" s="7" t="s">
         <v>147</v>
-      </c>
-      <c r="F46" s="7" t="s">
-        <v>148</v>
       </c>
       <c r="G46" s="14"/>
       <c r="H46" s="14"/>
@@ -2770,7 +2767,7 @@
     </row>
     <row r="47" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B47" s="28">
         <v>2017</v>
@@ -2780,7 +2777,7 @@
         <v>Vermont Academy Boys Lacrosse</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -2796,7 +2793,7 @@
     </row>
     <row r="48" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B48" s="28">
         <v>2017</v>
@@ -2806,7 +2803,7 @@
         <v>Kents Hill Boys Lacrosse</v>
       </c>
       <c r="D48" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="14"/>
@@ -2822,7 +2819,7 @@
     </row>
     <row r="49" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" s="28">
         <v>2017</v>
@@ -2832,13 +2829,13 @@
         <v>Berwick Academy Boys Lacrosse</v>
       </c>
       <c r="D49" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>154</v>
       </c>
-      <c r="E49" s="7" t="s">
+      <c r="F49" s="7" t="s">
         <v>155</v>
-      </c>
-      <c r="F49" s="7" t="s">
-        <v>156</v>
       </c>
       <c r="G49" s="14"/>
       <c r="H49" s="14"/>
@@ -2852,7 +2849,7 @@
     </row>
     <row r="50" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B50" s="28">
         <v>2017</v>
@@ -2862,10 +2859,10 @@
         <v>Canterbury School Boys Lacrosse</v>
       </c>
       <c r="D50" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="E50" s="7" t="s">
         <v>158</v>
-      </c>
-      <c r="E50" s="7" t="s">
-        <v>159</v>
       </c>
       <c r="F50" s="14"/>
       <c r="G50" s="14"/>
@@ -2880,7 +2877,7 @@
     </row>
     <row r="51" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B51" s="28">
         <v>2017</v>
@@ -2890,7 +2887,7 @@
         <v>Hoosac School Boys Lacrosse</v>
       </c>
       <c r="D51" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
@@ -2906,7 +2903,7 @@
     </row>
     <row r="52" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B52" s="28">
         <v>2017</v>
@@ -2916,10 +2913,10 @@
         <v>St. George's School Boys Lacrosse</v>
       </c>
       <c r="D52" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="E52" s="7" t="s">
         <v>163</v>
-      </c>
-      <c r="E52" s="7" t="s">
-        <v>164</v>
       </c>
       <c r="F52" s="14"/>
       <c r="G52" s="14"/>
@@ -2934,7 +2931,7 @@
     </row>
     <row r="53" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B53" s="28">
         <v>2017</v>
@@ -2944,13 +2941,13 @@
         <v>Hill School Boys Lacrosse</v>
       </c>
       <c r="D53" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>165</v>
       </c>
-      <c r="E53" s="7" t="s">
+      <c r="F53" s="7" t="s">
         <v>166</v>
-      </c>
-      <c r="F53" s="7" t="s">
-        <v>167</v>
       </c>
       <c r="G53" s="14"/>
       <c r="H53" s="14"/>
@@ -2964,7 +2961,7 @@
     </row>
     <row r="54" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B54" s="28">
         <v>2017</v>
@@ -2974,7 +2971,7 @@
         <v>Pingree School Boys Lacrosse</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -2990,7 +2987,7 @@
     </row>
     <row r="55" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="4" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B55" s="28">
         <v>2017</v>
@@ -3000,13 +2997,13 @@
         <v>Lawrenceville School Boys Lacrosse</v>
       </c>
       <c r="D55" s="7" t="s">
+        <v>169</v>
+      </c>
+      <c r="E55" s="7" t="s">
         <v>170</v>
       </c>
-      <c r="E55" s="7" t="s">
+      <c r="F55" s="7" t="s">
         <v>171</v>
-      </c>
-      <c r="F55" s="7" t="s">
-        <v>172</v>
       </c>
       <c r="G55" s="14"/>
       <c r="H55" s="14"/>
@@ -3020,7 +3017,7 @@
     </row>
     <row r="56" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B56" s="28">
         <v>2017</v>
@@ -3030,7 +3027,7 @@
         <v>North Yarmouth Academy Boys Lacrosse</v>
       </c>
       <c r="D56" s="7" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="14"/>
@@ -3046,7 +3043,7 @@
     </row>
     <row r="57" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A57" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B57" s="28">
         <v>2017</v>
@@ -3056,13 +3053,13 @@
         <v>Princeton Day School Boys Lacrosse</v>
       </c>
       <c r="D57" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="E57" s="7" t="s">
         <v>175</v>
       </c>
-      <c r="E57" s="7" t="s">
+      <c r="F57" s="7" t="s">
         <v>176</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>177</v>
       </c>
       <c r="G57" s="14"/>
       <c r="H57" s="14"/>
@@ -3076,7 +3073,7 @@
     </row>
     <row r="58" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A58" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B58" s="28">
         <v>2017</v>
@@ -3086,13 +3083,13 @@
         <v>Middlesex Boys Lacrosse</v>
       </c>
       <c r="D58" s="7" t="s">
+        <v>178</v>
+      </c>
+      <c r="E58" s="7" t="s">
         <v>179</v>
       </c>
-      <c r="E58" s="7" t="s">
+      <c r="F58" s="7" t="s">
         <v>180</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>181</v>
       </c>
       <c r="G58" s="14"/>
       <c r="H58" s="14"/>
@@ -3106,7 +3103,7 @@
     </row>
     <row r="59" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A59" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B59" s="28">
         <v>2017</v>
@@ -3116,7 +3113,7 @@
         <v>Brewster Academy Boys Lacrosse</v>
       </c>
       <c r="D59" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E59" s="14"/>
       <c r="F59" s="14"/>
@@ -3132,7 +3129,7 @@
     </row>
     <row r="60" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A60" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B60" s="28">
         <v>2017</v>
@@ -3142,13 +3139,13 @@
         <v>Worcester Academy Boys Lacrosse</v>
       </c>
       <c r="D60" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="E60" s="7" t="s">
         <v>185</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="F60" s="7" t="s">
         <v>186</v>
-      </c>
-      <c r="F60" s="7" t="s">
-        <v>187</v>
       </c>
       <c r="G60" s="14"/>
       <c r="H60" s="14"/>
@@ -3162,7 +3159,7 @@
     </row>
     <row r="61" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A61" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B61" s="28">
         <v>2017</v>
@@ -3172,7 +3169,7 @@
         <v>Moses Brown Boys Lacrosse</v>
       </c>
       <c r="D61" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E61" s="14"/>
       <c r="F61" s="14"/>
@@ -3188,7 +3185,7 @@
     </row>
     <row r="62" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A62" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B62" s="28">
         <v>2017</v>
@@ -3198,7 +3195,7 @@
         <v>Portsmouth Abbey Boys Lacrosse</v>
       </c>
       <c r="D62" s="7" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E62" s="14"/>
       <c r="F62" s="14"/>
@@ -3214,7 +3211,7 @@
     </row>
     <row r="63" spans="1:13" ht="13" x14ac:dyDescent="0.15">
       <c r="A63" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B63" s="28">
         <v>2017</v>
@@ -3224,13 +3221,13 @@
         <v>Kingswood-Oxford Boys Lacrosse</v>
       </c>
       <c r="D63" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="E63" s="7" t="s">
         <v>193</v>
       </c>
-      <c r="E63" s="7" t="s">
+      <c r="F63" s="7" t="s">
         <v>194</v>
-      </c>
-      <c r="F63" s="7" t="s">
-        <v>195</v>
       </c>
       <c r="G63" s="14"/>
       <c r="H63" s="14"/>
@@ -17435,10 +17432,10 @@
         <v>Lawrence Academy Girls Lacrosse</v>
       </c>
       <c r="D2" s="17" t="s">
+        <v>195</v>
+      </c>
+      <c r="E2" s="17" t="s">
         <v>196</v>
-      </c>
-      <c r="E2" s="17" t="s">
-        <v>197</v>
       </c>
       <c r="F2" s="17"/>
       <c r="G2" s="18" t="s">
@@ -17457,13 +17454,13 @@
         <v>Dexter Southfield Girls Lacrosse</v>
       </c>
       <c r="D3" s="18" t="s">
+        <v>197</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>198</v>
       </c>
-      <c r="E3" s="18" t="s">
+      <c r="F3" s="18" t="s">
         <v>199</v>
-      </c>
-      <c r="F3" s="18" t="s">
-        <v>200</v>
       </c>
       <c r="G3" s="20" t="s">
         <v>8</v>
@@ -17481,7 +17478,7 @@
         <v>Kimball Union Academy Girls Lacrosse</v>
       </c>
       <c r="D4" s="17" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="E4" s="17"/>
       <c r="F4" s="21"/>
@@ -17501,10 +17498,10 @@
         <v>Rivers School Girls Lacrosse</v>
       </c>
       <c r="D5" s="17" t="s">
+        <v>201</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>202</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>203</v>
       </c>
       <c r="F5" s="22"/>
       <c r="G5" s="18" t="s">
@@ -17523,7 +17520,7 @@
         <v>Phillips Exeter Academy Lacrosse</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E6" s="24"/>
       <c r="F6" s="25"/>
@@ -17543,13 +17540,13 @@
         <v>Thayer Academy Girls Lacrosse</v>
       </c>
       <c r="D7" s="18" t="s">
+        <v>204</v>
+      </c>
+      <c r="E7" s="18" t="s">
         <v>205</v>
       </c>
-      <c r="E7" s="18" t="s">
+      <c r="F7" s="18" t="s">
         <v>206</v>
-      </c>
-      <c r="F7" s="18" t="s">
-        <v>207</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>8</v>
@@ -17567,10 +17564,10 @@
         <v>The Gunnery School Girls Lacrosse</v>
       </c>
       <c r="D8" s="18" t="s">
+        <v>207</v>
+      </c>
+      <c r="E8" s="18" t="s">
         <v>208</v>
-      </c>
-      <c r="E8" s="18" t="s">
-        <v>209</v>
       </c>
       <c r="F8" s="25"/>
       <c r="G8" s="18" t="s">
@@ -17579,7 +17576,7 @@
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="32" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B9" s="28">
         <v>2017</v>
@@ -17589,7 +17586,7 @@
         <v>Nichols School Girls Lacrosse</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E9" s="25"/>
       <c r="F9" s="25"/>
@@ -17599,7 +17596,7 @@
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="4" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B10" s="28">
         <v>2017</v>
@@ -17609,7 +17606,7 @@
         <v>Phillips Andover Academy Girls Lacrosse</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
@@ -17619,7 +17616,7 @@
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="28">
         <v>2017</v>
@@ -17629,10 +17626,10 @@
         <v>Taft School Girls Lacrosse</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>213</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>214</v>
       </c>
       <c r="F11" s="14"/>
       <c r="G11" s="7" t="s">
@@ -17641,7 +17638,7 @@
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B12" s="28">
         <v>2017</v>
@@ -17651,10 +17648,10 @@
         <v>Albany Academy Girls Lacrosse</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>214</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>215</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>216</v>
       </c>
       <c r="F12" s="14"/>
       <c r="G12" s="7" t="s">
@@ -17663,7 +17660,7 @@
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B13" s="28">
         <v>2017</v>
@@ -17673,13 +17670,13 @@
         <v>Proctor Academy Girls Lacrosse</v>
       </c>
       <c r="D13" s="7" t="s">
+        <v>216</v>
+      </c>
+      <c r="E13" s="7" t="s">
         <v>217</v>
       </c>
-      <c r="E13" s="7" t="s">
+      <c r="F13" s="7" t="s">
         <v>218</v>
-      </c>
-      <c r="F13" s="7" t="s">
-        <v>219</v>
       </c>
       <c r="G13" s="7" t="s">
         <v>8</v>
@@ -17687,7 +17684,7 @@
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="28">
         <v>2017</v>
@@ -17697,7 +17694,7 @@
         <v>Milton Academy Girls Lacrosse</v>
       </c>
       <c r="D14" s="7" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E14" s="14"/>
       <c r="F14" s="14"/>
@@ -17707,7 +17704,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B15" s="28">
         <v>2017</v>
@@ -17717,10 +17714,10 @@
         <v>New Hampton School Girls Lacrosse</v>
       </c>
       <c r="D15" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E15" s="7" t="s">
         <v>221</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>222</v>
       </c>
       <c r="F15" s="14"/>
       <c r="G15" s="7" t="s">
@@ -17729,7 +17726,7 @@
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B16" s="28">
         <v>2017</v>
@@ -17739,13 +17736,13 @@
         <v>Winchendon School Girls Lacrosse</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="E16" s="7" t="s">
         <v>223</v>
       </c>
-      <c r="E16" s="7" t="s">
+      <c r="F16" s="7" t="s">
         <v>224</v>
-      </c>
-      <c r="F16" s="7" t="s">
-        <v>225</v>
       </c>
       <c r="G16" s="7" t="s">
         <v>8</v>
@@ -17753,7 +17750,7 @@
     </row>
     <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B17" s="28">
         <v>2017</v>
@@ -17763,10 +17760,10 @@
         <v>Loomis-Chaffee Girls Lacrosse</v>
       </c>
       <c r="D17" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="E17" s="7" t="s">
         <v>226</v>
-      </c>
-      <c r="E17" s="7" t="s">
-        <v>227</v>
       </c>
       <c r="F17" s="14"/>
       <c r="G17" s="7" t="s">
@@ -17775,7 +17772,7 @@
     </row>
     <row r="18" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="28">
         <v>2017</v>
@@ -17785,10 +17782,10 @@
         <v>Tabor Academy Girls Lacrosse</v>
       </c>
       <c r="D18" s="7" t="s">
+        <v>227</v>
+      </c>
+      <c r="E18" s="7" t="s">
         <v>228</v>
-      </c>
-      <c r="E18" s="7" t="s">
-        <v>229</v>
       </c>
       <c r="F18" s="14"/>
       <c r="G18" s="7" t="s">
@@ -17797,7 +17794,7 @@
     </row>
     <row r="19" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B19" s="28">
         <v>2017</v>
@@ -17807,7 +17804,7 @@
         <v>Tilton School Girls Lacrosse</v>
       </c>
       <c r="D19" s="7" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E19" s="14"/>
       <c r="F19" s="14"/>
@@ -17817,7 +17814,7 @@
     </row>
     <row r="20" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="8" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B20" s="28">
         <v>2017</v>
@@ -17827,7 +17824,7 @@
         <v>Kent School Girls Lacrosse</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="E20" s="14"/>
       <c r="F20" s="14"/>
@@ -17837,7 +17834,7 @@
     </row>
     <row r="21" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B21" s="28">
         <v>2017</v>
@@ -17847,13 +17844,13 @@
         <v>Cushing Academy Girls Lacrosse</v>
       </c>
       <c r="D21" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="E21" s="7" t="s">
         <v>232</v>
       </c>
-      <c r="E21" s="7" t="s">
+      <c r="F21" s="7" t="s">
         <v>233</v>
-      </c>
-      <c r="F21" s="7" t="s">
-        <v>234</v>
       </c>
       <c r="G21" s="7" t="s">
         <v>8</v>
@@ -17861,7 +17858,7 @@
     </row>
     <row r="22" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A22" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B22" s="28">
         <v>2017</v>
@@ -17871,7 +17868,7 @@
         <v>Pomfret School Girls Lacrosse</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
@@ -17881,7 +17878,7 @@
     </row>
     <row r="23" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A23" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B23" s="28">
         <v>2017</v>
@@ -17891,7 +17888,7 @@
         <v>Berkshire School Girls Lacrosse</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
@@ -17901,7 +17898,7 @@
     </row>
     <row r="24" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B24" s="28">
         <v>2017</v>
@@ -17911,7 +17908,7 @@
         <v>Holderness School Girls Lacrosse</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
@@ -17921,7 +17918,7 @@
     </row>
     <row r="25" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="28">
         <v>2017</v>
@@ -17931,10 +17928,10 @@
         <v>Westminster School Girls Lacrosse</v>
       </c>
       <c r="D25" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="E25" s="7" t="s">
         <v>238</v>
-      </c>
-      <c r="E25" s="7" t="s">
-        <v>239</v>
       </c>
       <c r="F25" s="14"/>
       <c r="G25" s="7" t="s">
@@ -17943,7 +17940,7 @@
     </row>
     <row r="26" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="8" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B26" s="28">
         <v>2017</v>
@@ -17953,13 +17950,13 @@
         <v>Millbrook School Girls Lacrosse</v>
       </c>
       <c r="D26" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="E26" s="7" t="s">
         <v>240</v>
       </c>
-      <c r="E26" s="7" t="s">
+      <c r="F26" s="7" t="s">
         <v>241</v>
-      </c>
-      <c r="F26" s="7" t="s">
-        <v>242</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>8</v>
@@ -17967,7 +17964,7 @@
     </row>
     <row r="27" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B27" s="28">
         <v>2017</v>
@@ -17977,13 +17974,13 @@
         <v>Williston-Northampton Girls Lacrosse</v>
       </c>
       <c r="D27" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="E27" s="7" t="s">
         <v>243</v>
       </c>
-      <c r="E27" s="7" t="s">
+      <c r="F27" s="7" t="s">
         <v>244</v>
-      </c>
-      <c r="F27" s="7" t="s">
-        <v>245</v>
       </c>
       <c r="G27" s="7" t="s">
         <v>8</v>
@@ -17991,7 +17988,7 @@
     </row>
     <row r="28" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A28" s="4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B28" s="28">
         <v>2017</v>
@@ -18001,10 +17998,10 @@
         <v>Deerfield Academy Girls Lacrosse</v>
       </c>
       <c r="D28" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="E28" s="7" t="s">
         <v>246</v>
-      </c>
-      <c r="E28" s="7" t="s">
-        <v>247</v>
       </c>
       <c r="F28" s="14"/>
       <c r="G28" s="7" t="s">
@@ -18013,7 +18010,7 @@
     </row>
     <row r="29" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A29" s="8" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B29" s="28">
         <v>2017</v>
@@ -18023,7 +18020,7 @@
         <v>Noble &amp; Greenough Girls Lacrosse</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
@@ -18033,7 +18030,7 @@
     </row>
     <row r="30" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A30" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B30" s="28">
         <v>2017</v>
@@ -18043,7 +18040,7 @@
         <v>Hotchkiss School Girls Lacrosse</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="E30" s="14"/>
       <c r="F30" s="14"/>
@@ -18053,7 +18050,7 @@
     </row>
     <row r="31" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="8" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B31" s="28">
         <v>2017</v>
@@ -18063,10 +18060,10 @@
         <v>St. Paul's Girls Lacrosse</v>
       </c>
       <c r="D31" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="E31" s="7" t="s">
         <v>250</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>251</v>
       </c>
       <c r="F31" s="14"/>
       <c r="G31" s="7" t="s">
@@ -18075,7 +18072,7 @@
     </row>
     <row r="32" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B32" s="28">
         <v>2017</v>
@@ -18085,7 +18082,7 @@
         <v>Governor's Academy Girls Lacrosse</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="E32" s="14"/>
       <c r="F32" s="14"/>
@@ -18095,7 +18092,7 @@
     </row>
     <row r="33" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="8" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B33" s="28">
         <v>2017</v>
@@ -18105,10 +18102,10 @@
         <v>Groton School Girls Lacrosse</v>
       </c>
       <c r="D33" s="7" t="s">
+        <v>252</v>
+      </c>
+      <c r="E33" s="7" t="s">
         <v>253</v>
-      </c>
-      <c r="E33" s="7" t="s">
-        <v>254</v>
       </c>
       <c r="F33" s="14"/>
       <c r="G33" s="7" t="s">
@@ -18117,7 +18114,7 @@
     </row>
     <row r="34" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B34" s="28">
         <v>2017</v>
@@ -18127,7 +18124,7 @@
         <v>St. Mark's Girls Lacrosse</v>
       </c>
       <c r="D34" s="7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E34" s="14"/>
       <c r="F34" s="14"/>
@@ -18137,7 +18134,7 @@
     </row>
     <row r="35" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="8" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B35" s="28">
         <v>2017</v>
@@ -18147,10 +18144,10 @@
         <v>Choate Girls Lacrosse</v>
       </c>
       <c r="D35" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="E35" s="7" t="s">
         <v>256</v>
-      </c>
-      <c r="E35" s="7" t="s">
-        <v>257</v>
       </c>
       <c r="F35" s="14"/>
       <c r="G35" s="7" t="s">
@@ -18159,7 +18156,7 @@
     </row>
     <row r="36" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B36" s="28">
         <v>2017</v>
@@ -18169,7 +18166,7 @@
         <v>BB&amp;N Girls Lacrosse</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="E36" s="14"/>
       <c r="F36" s="14"/>
@@ -18179,7 +18176,7 @@
     </row>
     <row r="37" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="8" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B37" s="28">
         <v>2017</v>
@@ -18189,7 +18186,7 @@
         <v>Hebron Academy Girls Lacrosse</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E37" s="14"/>
       <c r="F37" s="14"/>
@@ -18199,7 +18196,7 @@
     </row>
     <row r="38" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="8" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B38" s="28">
         <v>2017</v>
@@ -18209,13 +18206,13 @@
         <v>Brooks School Girls Lacrosse</v>
       </c>
       <c r="D38" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E38" s="7" t="s">
         <v>260</v>
       </c>
-      <c r="E38" s="7" t="s">
+      <c r="F38" s="7" t="s">
         <v>261</v>
-      </c>
-      <c r="F38" s="7" t="s">
-        <v>262</v>
       </c>
       <c r="G38" s="7" t="s">
         <v>8</v>
@@ -18223,7 +18220,7 @@
     </row>
     <row r="39" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B39" s="28">
         <v>2017</v>
@@ -18233,13 +18230,13 @@
         <v>Northfield - Mt Hermon Girls Lacrosse</v>
       </c>
       <c r="D39" s="7" t="s">
+        <v>262</v>
+      </c>
+      <c r="E39" s="7" t="s">
         <v>263</v>
       </c>
-      <c r="E39" s="7" t="s">
-        <v>264</v>
-      </c>
       <c r="F39" s="7" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G39" s="7" t="s">
         <v>8</v>
@@ -18247,7 +18244,7 @@
     </row>
     <row r="40" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="8" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B40" s="28">
         <v>2017</v>
@@ -18257,7 +18254,7 @@
         <v>Vermont Academy Girls Lacrosse</v>
       </c>
       <c r="D40" s="7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E40" s="14"/>
       <c r="F40" s="14"/>
@@ -18267,7 +18264,7 @@
     </row>
     <row r="41" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B41" s="28">
         <v>2017</v>
@@ -18277,7 +18274,7 @@
         <v>Kents Hill Girls Lacrosse</v>
       </c>
       <c r="D41" s="7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="E41" s="14"/>
       <c r="F41" s="14"/>
@@ -18287,7 +18284,7 @@
     </row>
     <row r="42" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="8" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B42" s="28">
         <v>2017</v>
@@ -18297,13 +18294,13 @@
         <v>Berwick Academy Girls Lacrosse</v>
       </c>
       <c r="D42" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="E42" s="7" t="s">
         <v>267</v>
       </c>
-      <c r="E42" s="7" t="s">
+      <c r="F42" s="7" t="s">
         <v>268</v>
-      </c>
-      <c r="F42" s="7" t="s">
-        <v>269</v>
       </c>
       <c r="G42" s="7" t="s">
         <v>8</v>
@@ -18311,7 +18308,7 @@
     </row>
     <row r="43" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B43" s="28">
         <v>2017</v>
@@ -18321,10 +18318,10 @@
         <v>Canterbury School Girls Lacrosse</v>
       </c>
       <c r="D43" s="7" t="s">
+        <v>269</v>
+      </c>
+      <c r="E43" s="7" t="s">
         <v>270</v>
-      </c>
-      <c r="E43" s="7" t="s">
-        <v>271</v>
       </c>
       <c r="F43" s="14"/>
       <c r="G43" s="7" t="s">
@@ -18333,7 +18330,7 @@
     </row>
     <row r="44" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="8" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B44" s="28">
         <v>2017</v>
@@ -18343,7 +18340,7 @@
         <v>Hoosac School Girls Lacrosse</v>
       </c>
       <c r="D44" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="14"/>
@@ -18353,7 +18350,7 @@
     </row>
     <row r="45" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B45" s="28">
         <v>2017</v>
@@ -18363,13 +18360,13 @@
         <v>St. George's School Girls Lacrosse</v>
       </c>
       <c r="D45" s="7" t="s">
+        <v>271</v>
+      </c>
+      <c r="E45" s="7" t="s">
         <v>272</v>
       </c>
-      <c r="E45" s="7" t="s">
+      <c r="F45" s="7" t="s">
         <v>273</v>
-      </c>
-      <c r="F45" s="7" t="s">
-        <v>274</v>
       </c>
       <c r="G45" s="7" t="s">
         <v>8</v>
@@ -18377,7 +18374,7 @@
     </row>
     <row r="46" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="33" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B46" s="28">
         <v>2017</v>
@@ -18387,10 +18384,10 @@
         <v>Hill School Girls Lacrosse</v>
       </c>
       <c r="D46" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="E46" s="7" t="s">
         <v>275</v>
-      </c>
-      <c r="E46" s="7" t="s">
-        <v>276</v>
       </c>
       <c r="F46" s="14"/>
       <c r="G46" s="7" t="s">
@@ -18399,7 +18396,7 @@
     </row>
     <row r="47" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B47" s="28">
         <v>2017</v>
@@ -18409,7 +18406,7 @@
         <v>Pingree School Girls Lacrosse</v>
       </c>
       <c r="D47" s="7" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="14"/>
@@ -18419,7 +18416,7 @@
     </row>
     <row r="48" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="31" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B48" s="28">
         <v>2017</v>
@@ -18429,13 +18426,13 @@
         <v>Lawrenceville School Girls Lacrosse</v>
       </c>
       <c r="D48" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="E48" s="7" t="s">
         <v>277</v>
       </c>
-      <c r="E48" s="7" t="s">
+      <c r="F48" s="7" t="s">
         <v>278</v>
-      </c>
-      <c r="F48" s="7" t="s">
-        <v>279</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>8</v>
@@ -18443,7 +18440,7 @@
     </row>
     <row r="49" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="8" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B49" s="28">
         <v>2017</v>
@@ -18453,10 +18450,10 @@
         <v>North Yarmouth Academy Girls Lacrosse</v>
       </c>
       <c r="D49" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="E49" s="7" t="s">
         <v>280</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>281</v>
       </c>
       <c r="F49" s="14"/>
       <c r="G49" s="7" t="s">
@@ -18465,7 +18462,7 @@
     </row>
     <row r="50" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="4" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B50" s="28">
         <v>2017</v>
@@ -18475,7 +18472,7 @@
         <v>Princeton Day School Girls Lacrosse</v>
       </c>
       <c r="D50" s="7" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="14"/>
@@ -18485,7 +18482,7 @@
     </row>
     <row r="51" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A51" s="8" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B51" s="28">
         <v>2017</v>
@@ -18495,10 +18492,10 @@
         <v>Middlesex Girls Lacrosse</v>
       </c>
       <c r="D51" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="E51" s="7" t="s">
         <v>283</v>
-      </c>
-      <c r="E51" s="7" t="s">
-        <v>284</v>
       </c>
       <c r="F51" s="14"/>
       <c r="G51" s="7" t="s">
@@ -18507,7 +18504,7 @@
     </row>
     <row r="52" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A52" s="4" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B52" s="28">
         <v>2017</v>
@@ -18517,7 +18514,7 @@
         <v>Brewster Academy Girls Lacrosse</v>
       </c>
       <c r="D52" s="7" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="14"/>
@@ -18527,7 +18524,7 @@
     </row>
     <row r="53" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A53" s="8" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B53" s="28">
         <v>2017</v>
@@ -18537,10 +18534,10 @@
         <v>Worcester Academy Girls Lacrosse</v>
       </c>
       <c r="D53" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="E53" s="7" t="s">
         <v>286</v>
-      </c>
-      <c r="E53" s="7" t="s">
-        <v>287</v>
       </c>
       <c r="F53" s="14"/>
       <c r="G53" s="7" t="s">
@@ -18549,7 +18546,7 @@
     </row>
     <row r="54" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A54" s="4" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B54" s="28">
         <v>2017</v>
@@ -18559,7 +18556,7 @@
         <v>Moses Brown Girls Lacrosse</v>
       </c>
       <c r="D54" s="7" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="14"/>
@@ -18569,7 +18566,7 @@
     </row>
     <row r="55" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A55" s="8" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B55" s="28">
         <v>2017</v>
@@ -18579,7 +18576,7 @@
         <v>Portsmouth Abbey Girls Lacrosse</v>
       </c>
       <c r="D55" s="7" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="14"/>
@@ -18589,7 +18586,7 @@
     </row>
     <row r="56" spans="1:7" ht="13" x14ac:dyDescent="0.15">
       <c r="A56" s="16" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B56" s="28">
         <v>2017</v>
@@ -18599,10 +18596,10 @@
         <v>Kingswood-Oxford Girls Lacrosse</v>
       </c>
       <c r="D56" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E56" s="7" t="s">
         <v>289</v>
-      </c>
-      <c r="E56" s="7" t="s">
-        <v>290</v>
       </c>
       <c r="F56" s="14"/>
       <c r="G56" s="7" t="s">

</xml_diff>